<commit_message>
Updates means of fig 2, 3, 4.
Updates means for 6 and 10 political cascades.
</commit_message>
<xml_diff>
--- a/Fig4 A-D.xlsx
+++ b/Fig4 A-D.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\alonsela\Dropbox\dropbox\Dropbox\_WORK_IN_PROGRESS\Ariel-Culs\article\PlosOne\git-filderLocal\tweets_politics_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alonsela\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187F2502-E454-4684-B134-C047ADB40573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{29B48F6D-8186-40BF-A1CB-D042AB14B21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="20376" windowHeight="12216" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fig4A_B" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
   <si>
     <t xml:space="preserve"> 'Venezuela Politics'</t>
   </si>
@@ -176,9 +176,6 @@
     <t xml:space="preserve">t-test Score </t>
   </si>
   <si>
-    <t xml:space="preserve">Fig 2 t-test </t>
-  </si>
-  <si>
     <t xml:space="preserve">t-test Fig 3 </t>
   </si>
   <si>
@@ -188,7 +185,19 @@
     <t>Hashtags</t>
   </si>
   <si>
-    <t>Mean</t>
+    <t>Mean (6 politics)</t>
+  </si>
+  <si>
+    <t>Mean (All politics)</t>
+  </si>
+  <si>
+    <t>Fig 2 t-test (ALL)</t>
+  </si>
+  <si>
+    <t>Mean (all)</t>
+  </si>
+  <si>
+    <t>Mean (6)</t>
   </si>
 </sst>
 </file>
@@ -196,7 +205,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
@@ -597,7 +606,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -964,6 +973,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1010,7 +1056,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1090,6 +1136,33 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="36" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="36" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="36" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="36" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="36" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1104,6 +1177,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1123,49 +1214,13 @@
     <xf numFmtId="0" fontId="22" fillId="35" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="36" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="36" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="36" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="36" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="36" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="36" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="36" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="36" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5897,10 +5952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S29"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5981,11 +6036,11 @@
       <c r="E4" s="16">
         <v>6.41</v>
       </c>
-      <c r="Q4" s="27" t="s">
+      <c r="Q4" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
     </row>
     <row r="5" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
@@ -6004,9 +6059,9 @@
       <c r="E5" s="16">
         <v>8.8000000000000007</v>
       </c>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="28"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
     </row>
     <row r="6" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
@@ -6025,9 +6080,9 @@
       <c r="E6" s="16">
         <v>2.54</v>
       </c>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="28"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
     </row>
     <row r="7" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
@@ -6046,9 +6101,9 @@
       <c r="E7" s="16">
         <v>16.036999999999999</v>
       </c>
-      <c r="Q7" s="28"/>
-      <c r="R7" s="28"/>
-      <c r="S7" s="28"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
@@ -6067,9 +6122,9 @@
       <c r="E8" s="16">
         <v>10.74</v>
       </c>
-      <c r="Q8" s="28"/>
-      <c r="R8" s="28"/>
-      <c r="S8" s="28"/>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="37"/>
+      <c r="S8" s="37"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
@@ -6088,9 +6143,9 @@
       <c r="E9" s="16">
         <v>10.29</v>
       </c>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="28"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="37"/>
     </row>
     <row r="10" spans="1:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
@@ -6109,9 +6164,9 @@
       <c r="E10" s="17">
         <v>5.43</v>
       </c>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="28"/>
-      <c r="S10" s="28"/>
+      <c r="Q10" s="37"/>
+      <c r="R10" s="37"/>
+      <c r="S10" s="37"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
@@ -6130,9 +6185,9 @@
       <c r="E11" s="15">
         <v>0.504</v>
       </c>
-      <c r="Q11" s="28"/>
-      <c r="R11" s="28"/>
-      <c r="S11" s="28"/>
+      <c r="Q11" s="37"/>
+      <c r="R11" s="37"/>
+      <c r="S11" s="37"/>
     </row>
     <row r="12" spans="1:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
@@ -6151,9 +6206,9 @@
       <c r="E12" s="16">
         <v>0.61</v>
       </c>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="28"/>
-      <c r="S12" s="28"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="37"/>
     </row>
     <row r="13" spans="1:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
@@ -6172,11 +6227,11 @@
       <c r="E13" s="16">
         <v>0.54300000000000004</v>
       </c>
-      <c r="Q13" s="29" t="s">
+      <c r="Q13" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="R13" s="30"/>
-      <c r="S13" s="31"/>
+      <c r="R13" s="39"/>
+      <c r="S13" s="40"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
@@ -6240,10 +6295,10 @@
       <c r="C19" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="39"/>
+      <c r="E19" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="42"/>
     </row>
     <row r="20" spans="2:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B20" s="23" t="s">
@@ -6253,8 +6308,8 @@
         <f>TTEST(D2:D10,D11:D16,2,2)</f>
         <v>1.4002383740079871E-5</v>
       </c>
-      <c r="E20" s="40"/>
-      <c r="F20" s="41"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="44"/>
     </row>
     <row r="21" spans="2:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B21" s="23" t="s">
@@ -6264,66 +6319,106 @@
         <f>TTEST(E2:E10,E11:E16,2,2)</f>
         <v>3.893263639096181E-4</v>
       </c>
-      <c r="E21" s="40"/>
-      <c r="F21" s="41"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="44"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E22" s="40"/>
-      <c r="F22" s="41"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="44"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E23" s="40"/>
-      <c r="F23" s="41"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="44"/>
     </row>
     <row r="24" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="23">
         <f>TTEST(D5:D10,D11:D16,2,2)</f>
         <v>4.3425462528849251E-5</v>
       </c>
-      <c r="E24" s="42"/>
-      <c r="F24" s="43"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="46"/>
     </row>
-    <row r="26" spans="2:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C27" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="45" t="str">
+    <row r="27" spans="2:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C28" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C29" s="30" t="str">
+        <f>C33</f>
+        <v>Politics</v>
+      </c>
+      <c r="D29" s="31">
+        <f>AVERAGE(D5:D10)</f>
+        <v>2.2075</v>
+      </c>
+      <c r="E29" s="31">
+        <f>AVERAGE(E5:E10)</f>
+        <v>8.9728333333333321</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="30" t="str">
+        <f>C34</f>
+        <v>Disaster</v>
+      </c>
+      <c r="D30" s="34">
+        <f>AVERAGE(D11:D16)</f>
+        <v>0.58849999999999991</v>
+      </c>
+      <c r="E30" s="34">
+        <f>AVERAGE(E11:E16)</f>
+        <v>0.52183333333333337</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="28" t="str">
         <f>D1</f>
         <v>Slope</v>
       </c>
-      <c r="E27" s="46" t="str">
+      <c r="E32" s="29" t="str">
         <f>E1</f>
         <v>Score</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C28" s="47" t="str">
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33" s="30" t="str">
         <f>C2</f>
         <v>Politics</v>
       </c>
-      <c r="D28" s="48">
+      <c r="D33" s="31">
         <f>AVERAGE(D2:D10)</f>
         <v>2.0566666666666666</v>
       </c>
-      <c r="E28" s="49">
+      <c r="E33" s="32">
         <f>AVERAGE(E2:E10)</f>
         <v>8.2007777777777768</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="50" t="str">
+    <row r="34" spans="3:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="33" t="str">
         <f>C11</f>
         <v>Disaster</v>
       </c>
-      <c r="D29" s="51">
+      <c r="D34" s="34">
         <f>AVERAGE(D11:D16)</f>
         <v>0.58849999999999991</v>
       </c>
-      <c r="E29" s="52">
+      <c r="E34" s="35">
         <f>AVERAGE(E11:E16)</f>
         <v>0.52183333333333337</v>
       </c>
@@ -6344,10 +6439,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -6691,13 +6786,13 @@
         <v>41</v>
       </c>
       <c r="C23" s="23">
-        <f>TTEST(D2:D12,D13:D18,2,2)</f>
-        <v>1.872381900160858E-3</v>
-      </c>
-      <c r="E23" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="33"/>
+        <f>TTEST(D2:D7,D13:D18,2,2)</f>
+        <v>4.1500471869407403E-3</v>
+      </c>
+      <c r="E23" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="48"/>
     </row>
     <row r="24" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B24" s="23" t="s">
@@ -6707,69 +6802,101 @@
         <f>TTEST(E2:E11,E13:E18,2,2)</f>
         <v>2.6474030264010025E-3</v>
       </c>
-      <c r="E24" s="34"/>
-      <c r="F24" s="35"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="50"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E25" s="34"/>
-      <c r="F25" s="35"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="50"/>
     </row>
     <row r="26" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="23" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C26" s="23">
-        <f>TTEST(D2:D7,D13:D18,2,2)</f>
-        <v>4.1500471869407403E-3</v>
-      </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="37"/>
+        <f>TTEST(D2:D12,D13:D18,2,2)</f>
+        <v>1.872381900160858E-3</v>
+      </c>
+      <c r="E26" s="51"/>
+      <c r="F26" s="52"/>
     </row>
     <row r="28" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C29" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="D29" s="45">
-        <f>D3</f>
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="E29" s="46">
-        <f>E3</f>
-        <v>1.3779999999999999</v>
-      </c>
+      <c r="C29" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="55"/>
+      <c r="E29" s="53"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C30" s="47" t="str">
+      <c r="C30" s="30" t="str">
         <f>C4</f>
         <v>Politics</v>
       </c>
-      <c r="D30" s="48">
+      <c r="D30" s="31">
+        <f>AVERAGE(D2:D7)</f>
+        <v>0.9378333333333333</v>
+      </c>
+      <c r="E30" s="32">
+        <f>AVERAGE(E2:E7)</f>
+        <v>1.2143333333333333</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="33" t="str">
+        <f>C13</f>
+        <v>Disaster</v>
+      </c>
+      <c r="D31" s="34">
+        <f>AVERAGE(D13:D18)</f>
+        <v>1.2078333333333333</v>
+      </c>
+      <c r="E31" s="35">
+        <f>AVERAGE(E13:E18)</f>
+        <v>2.1043333333333334</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="55"/>
+      <c r="E33" s="53"/>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="30" t="str">
+        <f>C8</f>
+        <v>Politics</v>
+      </c>
+      <c r="D34" s="31">
         <f>AVERAGE(D2:D12)</f>
         <v>0.9725454545454546</v>
       </c>
-      <c r="E30" s="48">
-        <f>AVERAGE(E2:E12)</f>
+      <c r="E34" s="32">
+        <f>AVERAGE(E2:E11)</f>
         <v>1.3894</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="50" t="str">
-        <f>C13</f>
+    <row r="35" spans="3:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="33" t="str">
+        <f>C17</f>
         <v>Disaster</v>
       </c>
-      <c r="D31" s="51">
+      <c r="D35" s="34">
         <f>AVERAGE(D13:D18)</f>
         <v>1.2078333333333333</v>
       </c>
-      <c r="E31" s="51">
+      <c r="E35" s="35">
         <f>AVERAGE(E13:E18)</f>
         <v>2.1043333333333334</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="E23:F26"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C33:E33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>